<commit_message>
Add Placement And Rack in Masterfile
</commit_message>
<xml_diff>
--- a/Equipment Tools.xlsx
+++ b/Equipment Tools.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
   <si>
     <t>Equipment and Tools Fields</t>
   </si>
@@ -59,28 +59,34 @@
     <t>Office / Department</t>
   </si>
   <si>
+    <t>Placement</t>
+  </si>
+  <si>
+    <t>Rack</t>
+  </si>
+  <si>
+    <t>Physical Condition</t>
+  </si>
+  <si>
     <t>Unit Cost</t>
   </si>
   <si>
     <t>Total Cost</t>
   </si>
   <si>
-    <t>Physical Condition</t>
-  </si>
-  <si>
     <t>Remarks</t>
   </si>
   <si>
     <t>Furniture, Fixtures and Equipment</t>
   </si>
   <si>
-    <t>FFE-TRA-BCD-1008</t>
+    <t>FFE-TRA-BCD-1011</t>
   </si>
   <si>
     <t>2019-04-23</t>
   </si>
   <si>
-    <t>test item</t>
+    <t>testing</t>
   </si>
   <si>
     <t>pc/s</t>
@@ -95,28 +101,28 @@
     <t>IT Department</t>
   </si>
   <si>
+    <t>test place</t>
+  </si>
+  <si>
+    <t>test rack</t>
+  </si>
+  <si>
     <t>12.00 USD</t>
   </si>
   <si>
-    <t>24 USD</t>
-  </si>
-  <si>
-    <t>Partially Damaged</t>
-  </si>
-  <si>
-    <t>FFE-TRA-BCD-1010</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>qq</t>
-  </si>
-  <si>
-    <t>qqqq</t>
-  </si>
-  <si>
     <t>12 USD</t>
+  </si>
+  <si>
+    <t>FFE-TRA-BCD-1013</t>
+  </si>
+  <si>
+    <t>sss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 </t>
   </si>
 </sst>
 </file>
@@ -499,7 +505,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,7 +513,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:19">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -515,7 +521,7 @@
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:19">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -567,114 +573,116 @@
       <c r="Q2" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="R2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:19">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="1">
+        <v>121</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1">
+        <v>112</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" s="1"/>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="1">
-        <v>123</v>
-      </c>
-      <c r="F3" s="1">
-        <v>123</v>
-      </c>
-      <c r="G3" s="1">
-        <v>123</v>
-      </c>
-      <c r="H3" s="1">
+      <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1">
         <v>2</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="J4" s="1"/>
+      <c r="K4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="L4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="M4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="A4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="1">
-        <v>1</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S4" s="1"/>
     </row>
   </sheetData>
   <sheetProtection sheet="true" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <protectedRanges>
-    <protectedRange name="pae1835ddb2e9e700070b1df9a4595e94" sqref="A3:Q3" password="C724"/>
-    <protectedRange name="p273ab5e3ecebbeb91396ca8354d6423e" sqref="A4:Q4" password="C724"/>
+    <protectedRange name="p6f5710c8199129451d13d7cdd4fbfe8e" sqref="A3:S3" password="C724"/>
+    <protectedRange name="p5789a9ca630561449388a885f4dbc751" sqref="A4:S4" password="C724"/>
   </protectedRanges>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add edit in available items
</commit_message>
<xml_diff>
--- a/Equipment Tools.xlsx
+++ b/Equipment Tools.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="203">
   <si>
     <t>Equipment and Tools Fields</t>
   </si>
@@ -80,142 +80,304 @@
     <t>Furniture, Fixtures and Equipment</t>
   </si>
   <si>
-    <t>FFE- COMP-BCD-1004</t>
-  </si>
-  <si>
-    <t>2019-04-16</t>
-  </si>
-  <si>
-    <t>Laptop AMD A9-9425 Radeon R5, 5 Compute cores 2C + 3G 3.10GHz 4GB RAM 64 Bit OS 500GB HDD</t>
-  </si>
-  <si>
-    <t>Asus</t>
-  </si>
-  <si>
-    <t>Asus VivoBook X540B</t>
-  </si>
-  <si>
-    <t>J6N0GR03E693245</t>
+    <t>FFE- COMP-BCD-1001</t>
+  </si>
+  <si>
+    <t>CPU Pentium, RAM(2GB), 64 Bit OS, 500GB HD</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>IT20190049</t>
   </si>
   <si>
     <t>pc/s</t>
   </si>
   <si>
-    <t>2019-04-17</t>
-  </si>
-  <si>
-    <t>Hennelen Tanan</t>
+    <t>Celina Marie Grabillo</t>
   </si>
   <si>
     <t>Assigned</t>
   </si>
   <si>
+    <t>EMG-Billing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 </t>
+  </si>
+  <si>
+    <t>FFE- COMP-BCD-1008</t>
+  </si>
+  <si>
+    <t>CPU Core i3, RAM(4GB), 64 Bit OS, x64 Based Processor</t>
+  </si>
+  <si>
+    <t>Neutron Lite</t>
+  </si>
+  <si>
+    <t>IT20190054</t>
+  </si>
+  <si>
+    <t>Zara Joy Gabales</t>
+  </si>
+  <si>
+    <t>FFE- COMP-BCD-1019</t>
+  </si>
+  <si>
+    <t>CPU, Core i5, RAM(4GB), 64 bit, x64 Based Processor, 500GB HDD</t>
+  </si>
+  <si>
+    <t>Fortress</t>
+  </si>
+  <si>
+    <t>IT20190099</t>
+  </si>
+  <si>
+    <t>Liza Marie Tasic</t>
+  </si>
+  <si>
+    <t>Shoppers Guide</t>
+  </si>
+  <si>
+    <t>FFE- COMP-BCD-1024</t>
+  </si>
+  <si>
+    <t>CPU,Core i5, 32 bit, x64 Based Processor 1TB HDD</t>
+  </si>
+  <si>
+    <t>IT20190176</t>
+  </si>
+  <si>
+    <t>Genie Saludo</t>
+  </si>
+  <si>
+    <t>HR/Admin</t>
+  </si>
+  <si>
+    <t>FFE- COMP-BCD-1031</t>
+  </si>
+  <si>
+    <t>Laptop Core i7-4610M CPU, RAM(8GB), 64 bit,x64 Based Processor</t>
+  </si>
+  <si>
+    <t>Toshiba</t>
+  </si>
+  <si>
+    <t>TECRA A50-A Series</t>
+  </si>
+  <si>
+    <t>PB654MAWGK7AE71</t>
+  </si>
+  <si>
+    <t>Ladi Bacong</t>
+  </si>
+  <si>
+    <t>FFE- COMP-BCD-1035</t>
+  </si>
+  <si>
+    <t>CPU, Core i3-4160, RAM(4GB), 64 bit, x64 Based Processor, 500GB HDD</t>
+  </si>
+  <si>
+    <t>Orion</t>
+  </si>
+  <si>
+    <t>IT20190343</t>
+  </si>
+  <si>
+    <t>Angelika Caballero</t>
+  </si>
+  <si>
+    <t>FFE- COMP-BCD-1036</t>
+  </si>
+  <si>
+    <t>CPU G3260 Intel Pentium, RAM(2GB), 32-bit OS, x64-based processor</t>
+  </si>
+  <si>
+    <t>IT20190345</t>
+  </si>
+  <si>
+    <t>Prency Francisco</t>
+  </si>
+  <si>
+    <t>FFE- COMP-BCD-1046</t>
+  </si>
+  <si>
+    <t>CPU Intel Core i3-4170, 4GB, 64bit-OS</t>
+  </si>
+  <si>
+    <t>Powerlogic</t>
+  </si>
+  <si>
+    <t>H81M-S1</t>
+  </si>
+  <si>
+    <t>IT20190399</t>
+  </si>
+  <si>
+    <t>Elaisa Jane Febrio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPU Core i3-4170, RAM(4GB), 64 bit, </t>
+  </si>
+  <si>
+    <t>ASUS</t>
+  </si>
+  <si>
+    <t>IT20190339</t>
+  </si>
+  <si>
+    <t>2019-05-07</t>
+  </si>
+  <si>
+    <t>Silena Jomiller</t>
+  </si>
+  <si>
+    <t>FFE- COMP-BCD-1053</t>
+  </si>
+  <si>
+    <t>CPU Intel Core i3-4170, 4GB, 64-bit OS</t>
+  </si>
+  <si>
+    <t>IT20190307</t>
+  </si>
+  <si>
+    <t>2019-09-02</t>
+  </si>
+  <si>
+    <t>Ruth Jan Destacamento</t>
+  </si>
+  <si>
+    <t>Accounting</t>
+  </si>
+  <si>
+    <t>FFE- COMP-BCD-1061</t>
+  </si>
+  <si>
+    <t>CPU Intel Core i3-4170 4GB 64-bit OS</t>
+  </si>
+  <si>
+    <t>IT20190108</t>
+  </si>
+  <si>
+    <t>Daisy Jane Sanchez</t>
+  </si>
+  <si>
+    <t>Trading</t>
+  </si>
+  <si>
+    <t>FFE- COMP-BCD-1062</t>
+  </si>
+  <si>
+    <t>CPU, Xeon, E3-1220, 64 bit, RAM(12GB), 1TB HDD and 500GB HDD</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>HP Proliant</t>
+  </si>
+  <si>
+    <t>CN65270AG4</t>
+  </si>
+  <si>
+    <t>Trading Department</t>
+  </si>
+  <si>
+    <t>FFE- COMP-BCD-1081</t>
+  </si>
+  <si>
+    <t>CPU Intel Core i3-4160 2GB RAM 32-bit OS</t>
+  </si>
+  <si>
+    <t>IT20190281</t>
+  </si>
+  <si>
+    <t>Teresa Tan</t>
+  </si>
+  <si>
+    <t>Contracts &amp; Compliance</t>
+  </si>
+  <si>
+    <t>FFE- COMP-BCD-1089</t>
+  </si>
+  <si>
+    <t>CPU Intel Core i3-4170 4GB RAM 64-bit OS</t>
+  </si>
+  <si>
+    <t>IT20190057</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>FFE- COMP-BCD-1093</t>
+  </si>
+  <si>
+    <t>Intel Core i3-4170 CPU @3.70GHz, 4GB RAM, 500GB HDD</t>
+  </si>
+  <si>
+    <t>ITBCD1033</t>
+  </si>
+  <si>
+    <t>Stephine David Severino</t>
+  </si>
+  <si>
     <t>IT Department</t>
   </si>
   <si>
-    <t xml:space="preserve">0.00 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 </t>
-  </si>
-  <si>
-    <t>FFE- COMP-BCD-1014</t>
-  </si>
-  <si>
-    <t>Laptop Core i7, RAM(4GB), 64 bit, x64 Based  Processor HDD 1TB</t>
-  </si>
-  <si>
-    <t>ASUS</t>
-  </si>
-  <si>
-    <t>X510U</t>
-  </si>
-  <si>
-    <t>J5NDCX11W504217</t>
-  </si>
-  <si>
-    <t>Carlos Antonio Leonardia</t>
-  </si>
-  <si>
-    <t>FFE- COMP-BCD-1031</t>
-  </si>
-  <si>
-    <t>Laptop Core i7-4610M CPU, RAM(8GB), 64 bit,x64 Based Processor</t>
-  </si>
-  <si>
-    <t>Toshiba</t>
-  </si>
-  <si>
-    <t>TECRA A50-A Series</t>
-  </si>
-  <si>
-    <t>PB654MAWGK7AE71</t>
-  </si>
-  <si>
-    <t>Ladi Bacong</t>
-  </si>
-  <si>
-    <t>Shoppers Guide</t>
-  </si>
-  <si>
-    <t>FFE- COMP-BCD-1074</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laptop 13.5 inches Intel Core i5-7200U, 4GB RAM, 64-bit OS </t>
+    <t>FFE- COMP-BCD-1094</t>
+  </si>
+  <si>
+    <t>CPU Intel Core i5-7400 4GB RAM 64-bit OS, 500gb HDD</t>
+  </si>
+  <si>
+    <t>IT20190288</t>
+  </si>
+  <si>
+    <t>2019-03-04</t>
+  </si>
+  <si>
+    <t>Aileen Tamano</t>
+  </si>
+  <si>
+    <t>FFE- COMP-BCD-1099</t>
+  </si>
+  <si>
+    <t>IT20190182</t>
+  </si>
+  <si>
+    <t>Syndey Sinoro</t>
+  </si>
+  <si>
+    <t>FFE- COMP-BCD-1105</t>
+  </si>
+  <si>
+    <t>Laptop 14inches, Intel Core i5-5200U CPU @ 2.20GHz, 4GB RAM, 1TB HDD</t>
   </si>
   <si>
     <t>Acer</t>
   </si>
   <si>
-    <t>Aspire E5-476G</t>
-  </si>
-  <si>
-    <t>NXGVSSP001820050D57600</t>
-  </si>
-  <si>
-    <t>Annavi Lacambra</t>
-  </si>
-  <si>
-    <t>Accounting</t>
-  </si>
-  <si>
-    <t>FFE- COMP-BCD-1078</t>
-  </si>
-  <si>
-    <t>Laptop Intel Celeron 2955U 4GB RAM 64-bit OS</t>
-  </si>
-  <si>
-    <t>Acer Aspire E1-432</t>
-  </si>
-  <si>
-    <t>Ma. Milagros Arana</t>
-  </si>
-  <si>
-    <t>Management</t>
-  </si>
-  <si>
-    <t>FFE- COMP-BCD-1105</t>
-  </si>
-  <si>
-    <t>Laptop 14inches, Intel Core i5-5200U CPU @ 2.20GHz, 4GB RAM, 1TB HDD</t>
-  </si>
-  <si>
     <t>NXV9USP018602033587600</t>
   </si>
   <si>
     <t>Jonah Faye Benares</t>
   </si>
   <si>
-    <t>FFE- COMP-BCD-1107</t>
-  </si>
-  <si>
-    <t>Laptop Charger</t>
-  </si>
-  <si>
-    <t>ADP-65VH D</t>
-  </si>
-  <si>
-    <t>6ARW53908NE</t>
+    <t>FFE- COMP-BCD-1111</t>
+  </si>
+  <si>
+    <t>Intel Core i5-7400 CPU @ 3.00Ghz, 4GB RAM, 500HDD</t>
+  </si>
+  <si>
+    <t>IT20190068</t>
+  </si>
+  <si>
+    <t>Jason Flor</t>
   </si>
   <si>
     <t>FFE- COMP-BCD-1118</t>
@@ -239,6 +401,30 @@
     <t>Borrowed</t>
   </si>
   <si>
+    <t>Intel Core i5-4460 CPU @ 3.20GHz, 8GB RAM, 1TB HDD</t>
+  </si>
+  <si>
+    <t>IT20190256</t>
+  </si>
+  <si>
+    <t>FFE- COMP-BCD-1125</t>
+  </si>
+  <si>
+    <t>IT20190340</t>
+  </si>
+  <si>
+    <t>FFE- COMP-BCD-1138</t>
+  </si>
+  <si>
+    <t>Intel Core i5-7400 CPU @3.00GHz, 4GB RAM, 500GB HDD</t>
+  </si>
+  <si>
+    <t>IT20190358</t>
+  </si>
+  <si>
+    <t>Rowena Ricarse</t>
+  </si>
+  <si>
     <t>FFE- COMP-BCD-1146</t>
   </si>
   <si>
@@ -254,25 +440,139 @@
     <t>2019-09-05</t>
   </si>
   <si>
-    <t>Available</t>
-  </si>
-  <si>
-    <t>FFE- COMP-BCD-1147</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laptop 12.5 inches Intel Core i5-4300U, 4GB RAM, 64-bit OS </t>
-  </si>
-  <si>
-    <t>dynabook R634/K</t>
-  </si>
-  <si>
-    <t>IT20190173</t>
-  </si>
-  <si>
-    <t>Rose Brenette Gaudite</t>
-  </si>
-  <si>
-    <t>Admin</t>
+    <t>FFE- COMP-BCD-1153</t>
+  </si>
+  <si>
+    <t>CPU core i5-7400 4GB(RAM), 64bit OS</t>
+  </si>
+  <si>
+    <t>NEUTRON ODYSSEY</t>
+  </si>
+  <si>
+    <t>IT20190020</t>
+  </si>
+  <si>
+    <t>Glenn Paul Toledo</t>
+  </si>
+  <si>
+    <t>FFE- COMP-BCD-1161</t>
+  </si>
+  <si>
+    <t>CPU intel(r) core i3-7100, 4GB (RAM</t>
+  </si>
+  <si>
+    <t>IT20190232</t>
+  </si>
+  <si>
+    <t>Zyndyryn Rosales</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>FFE- COMP-BCD-1166</t>
+  </si>
+  <si>
+    <t>CPU INTEL® CORE(TM) i3-7100, 4Gb (RAM), 64bit OS</t>
+  </si>
+  <si>
+    <t>IT20190073</t>
+  </si>
+  <si>
+    <t>2019-08-27</t>
+  </si>
+  <si>
+    <t>Crizeal Precious Marie Hilado</t>
+  </si>
+  <si>
+    <t>FFE- COMP-BCD-1174</t>
+  </si>
+  <si>
+    <t>IT20190162</t>
+  </si>
+  <si>
+    <t>Ladylyn Salavante</t>
+  </si>
+  <si>
+    <t>FFE- COMP-BCD-1175</t>
+  </si>
+  <si>
+    <t>CPU Intel Core i3-4150 4GB 64-bit OS</t>
+  </si>
+  <si>
+    <t>IT20190088</t>
+  </si>
+  <si>
+    <t>Marianita Tabilla</t>
+  </si>
+  <si>
+    <t>FFE- COMP-BCD-1183</t>
+  </si>
+  <si>
+    <t>CPU Intel ® Core™ i3-4150 CPU @ 3.50Ghz</t>
+  </si>
+  <si>
+    <t>Rise</t>
+  </si>
+  <si>
+    <t>IT-20190007</t>
+  </si>
+  <si>
+    <t>Krystal Gayle Tagalog</t>
+  </si>
+  <si>
+    <t>Add DDR3 2G/1333/2568 UL CL9 SN: 1014010MB0 ZPZB731825 (ZEPPELIN) as of August 08, 2019. - Hennelen Tanan &amp; Jason Flor</t>
+  </si>
+  <si>
+    <t>FFE- COMP-BCD-1185</t>
+  </si>
+  <si>
+    <t>CPU Intel Pentium G2020 2GB RAM 32-bit OS</t>
+  </si>
+  <si>
+    <t>IT2019086</t>
+  </si>
+  <si>
+    <t>Imelda Espera</t>
+  </si>
+  <si>
+    <t>Accounting / Finance</t>
+  </si>
+  <si>
+    <t>FFE- COMP-BCD-1194</t>
+  </si>
+  <si>
+    <t>CPU Inter® Pentium® CPU G2030 @ 3.00Ghz</t>
+  </si>
+  <si>
+    <t>IT20190370</t>
+  </si>
+  <si>
+    <t>Maylen Cabaylo</t>
+  </si>
+  <si>
+    <t>Purchasing</t>
+  </si>
+  <si>
+    <t>Remove DDR3 2G/1333/2568 UL CL9 SN: 1014010MB0 ZPZB731825 (ZEPPELIN) as of August 08, 2019. - Hennelen Tanan &amp; Jason Flor</t>
+  </si>
+  <si>
+    <t>FFE- COMP-BCD-1202</t>
+  </si>
+  <si>
+    <t>CPU INTEL® CORE™ i3-4170 @ 3.70Ghz</t>
+  </si>
+  <si>
+    <t>PowerLogic</t>
+  </si>
+  <si>
+    <t>IT20190059</t>
+  </si>
+  <si>
+    <t>Kervic Biñas</t>
+  </si>
+  <si>
+    <t>Replace VGA Cable to Glenn Paul as of 08-16-19 for compatibility purposes.</t>
   </si>
   <si>
     <t>FFE- COMP-BCD-1203</t>
@@ -287,49 +587,43 @@
     <t>IT20190045</t>
   </si>
   <si>
-    <t>2019-09-02</t>
-  </si>
-  <si>
     <t>Sherny Mago</t>
   </si>
   <si>
-    <t>FFE- COMP-BCD-1251</t>
-  </si>
-  <si>
-    <t>Laptop HP 15.6 2.10 GHz Intel Pentium Dual-Core Processor T4300 3GB DDR2 memory 320GB SATA hard drive Microsoft Windows 7 Home Premium Edition 64-bit</t>
-  </si>
-  <si>
-    <t>HP</t>
-  </si>
-  <si>
-    <t>G60-535DX</t>
-  </si>
-  <si>
-    <t>2CE9478DTJ</t>
-  </si>
-  <si>
-    <t>Old laptop of Sir butch Dujenio and charger is defective.</t>
-  </si>
-  <si>
-    <t>FFE- COMP-BCD-1253</t>
-  </si>
-  <si>
-    <t>Laptop Asus 14.0" Intel® Core™ i3 3217U	Processor Windows 8 Intel® HM76/HM70 Express Chipset DDR3 1600 MHz SDRAM, up to 4 G  500 GB Storage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASUS </t>
-  </si>
-  <si>
-    <t>X451C Notebook PC</t>
-  </si>
-  <si>
-    <t>E4N0CX061019148</t>
-  </si>
-  <si>
-    <t>2019-08-09</t>
-  </si>
-  <si>
-    <t>Old laptop of Miss Annavi Lacambra</t>
+    <t>FFE- COMP-BCD-1210</t>
+  </si>
+  <si>
+    <t>CPU INTEL® CORE™ i3-4160 @ 360Ghz</t>
+  </si>
+  <si>
+    <t>IT20190270</t>
+  </si>
+  <si>
+    <t>Gebby Jalandoni</t>
+  </si>
+  <si>
+    <t>FFE- COMP-BCD-1212</t>
+  </si>
+  <si>
+    <t>CPU Intel Core i3-7100 4GB 64-bit OS</t>
+  </si>
+  <si>
+    <t>IT20190035</t>
+  </si>
+  <si>
+    <t>Cristy Cesar</t>
+  </si>
+  <si>
+    <t>FFE- COMP-BCD-1219</t>
+  </si>
+  <si>
+    <t>CPU intel core i5</t>
+  </si>
+  <si>
+    <t>Mseries</t>
+  </si>
+  <si>
+    <t>IT20190136</t>
   </si>
 </sst>
 </file>
@@ -712,7 +1006,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:S15"/>
+  <dimension ref="A1:S39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -794,47 +1088,41 @@
       <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="1">
-        <v>1</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="L3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="S3" s="1"/>
     </row>
@@ -843,43 +1131,43 @@
         <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H4" s="1">
         <v>1</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M4" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="S4" s="1"/>
     </row>
@@ -888,45 +1176,43 @@
         <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>43</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H5" s="1">
         <v>1</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="S5" s="1"/>
     </row>
@@ -935,45 +1221,41 @@
         <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>50</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="H6" s="1">
         <v>1</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="S6" s="1"/>
     </row>
@@ -982,45 +1264,45 @@
         <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>49</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G7" s="1">
-        <v>34201363766</v>
+        <v>50</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="H7" s="1">
         <v>1</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="S7" s="1"/>
     </row>
@@ -1029,43 +1311,43 @@
         <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H8" s="1">
         <v>1</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="S8" s="1"/>
     </row>
@@ -1074,45 +1356,43 @@
         <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>65</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H9" s="1">
         <v>1</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="S9" s="1"/>
     </row>
@@ -1121,43 +1401,45 @@
         <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H10" s="1">
         <v>1</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="M10" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="S10" s="1"/>
     </row>
@@ -1166,43 +1448,43 @@
         <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>76</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="H11" s="1">
         <v>1</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K11" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="L11" s="1" t="s">
-        <v>79</v>
+        <v>27</v>
       </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="S11" s="1"/>
     </row>
@@ -1211,45 +1493,47 @@
         <v>20</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="H12" s="1">
         <v>1</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J12" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="K12" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="S12" s="1"/>
     </row>
@@ -1258,47 +1542,41 @@
         <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>88</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="H13" s="1">
         <v>1</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>90</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="S13" s="1"/>
     </row>
@@ -1307,96 +1585,1150 @@
         <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="H14" s="1">
         <v>1</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
+      <c r="K14" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="L14" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>46</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="S14" s="1" t="s">
-        <v>97</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:19">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>101</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="H15" s="1">
         <v>1</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="K15" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="L15" s="1" t="s">
-        <v>79</v>
+        <v>27</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="S15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S15" s="1"/>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S16" s="1"/>
+    </row>
+    <row r="17" spans="1:19">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S17" s="1"/>
+    </row>
+    <row r="18" spans="1:19">
+      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>104</v>
       </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S18" s="1"/>
+    </row>
+    <row r="19" spans="1:19">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S19" s="1"/>
+    </row>
+    <row r="20" spans="1:19">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H20" s="1">
+        <v>1</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S20" s="1"/>
+    </row>
+    <row r="21" spans="1:19">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H21" s="1">
+        <v>1</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S21" s="1"/>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S22" s="1"/>
+    </row>
+    <row r="23" spans="1:19">
+      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S23" s="1"/>
+    </row>
+    <row r="24" spans="1:19">
+      <c r="A24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H24" s="1">
+        <v>1</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S24" s="1"/>
+    </row>
+    <row r="25" spans="1:19">
+      <c r="A25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S25" s="1"/>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="A26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S26" s="1"/>
+    </row>
+    <row r="27" spans="1:19">
+      <c r="A27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S27" s="1"/>
+    </row>
+    <row r="28" spans="1:19">
+      <c r="A28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S28" s="1"/>
+    </row>
+    <row r="29" spans="1:19">
+      <c r="A29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H29" s="1">
+        <v>1</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R29" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S29" s="1"/>
+    </row>
+    <row r="30" spans="1:19">
+      <c r="A30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H30" s="1">
+        <v>1</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R30" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S30" s="1"/>
+    </row>
+    <row r="31" spans="1:19">
+      <c r="A31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H31" s="1">
+        <v>1</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R31" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S31" s="1"/>
+    </row>
+    <row r="32" spans="1:19">
+      <c r="A32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H32" s="1">
+        <v>1</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R32" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S32" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19">
+      <c r="A33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H33" s="1">
+        <v>1</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R33" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S33" s="1"/>
+    </row>
+    <row r="34" spans="1:19">
+      <c r="A34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="H34" s="1">
+        <v>1</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R34" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S34" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19">
+      <c r="A35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H35" s="1">
+        <v>1</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R35" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19">
+      <c r="A36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H36" s="1">
+        <v>1</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R36" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S36" s="1"/>
+    </row>
+    <row r="37" spans="1:19">
+      <c r="A37" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="H37" s="1">
+        <v>1</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R37" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S37" s="1"/>
+    </row>
+    <row r="38" spans="1:19">
+      <c r="A38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="H38" s="1">
+        <v>1</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R38" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S38" s="1"/>
+    </row>
+    <row r="39" spans="1:19">
+      <c r="A39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H39" s="1">
+        <v>1</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R39" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S39" s="1"/>
     </row>
   </sheetData>
   <sheetProtection sheet="true" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
@@ -1414,6 +2746,30 @@
     <protectedRange name="p8266175524bdc3373c732f49af634b83" sqref="A13:S13" password="C724"/>
     <protectedRange name="p425baa74d18709128e507f8e6d0cbd85" sqref="A14:S14" password="C724"/>
     <protectedRange name="p6c1a2fa7e1523769eaed853560e7974c" sqref="A15:S15" password="C724"/>
+    <protectedRange name="pafc6c1a6c7d1e22803599e859d3fb93b" sqref="A16:S16" password="C724"/>
+    <protectedRange name="p096f250de1417cdc958e8d9ae099f98d" sqref="A17:S17" password="C724"/>
+    <protectedRange name="p91983fd3ca885e7edfe78c22505189d1" sqref="A18:S18" password="C724"/>
+    <protectedRange name="p5dcef0a72b751c95e2fd6264de4125b4" sqref="A19:S19" password="C724"/>
+    <protectedRange name="p1953ab90313db9f64a8c5e36d530fd0b" sqref="A20:S20" password="C724"/>
+    <protectedRange name="pb334a9ca5b9771faf5894ce0a2b97f03" sqref="A21:S21" password="C724"/>
+    <protectedRange name="p17ca386c2586becaa1540f7bf057f3d6" sqref="A22:S22" password="C724"/>
+    <protectedRange name="p50542757ea57198cb7ef262ebc9ce1e7" sqref="A23:S23" password="C724"/>
+    <protectedRange name="p19411e35c40de284bd75d4cc4b5436fd" sqref="A24:S24" password="C724"/>
+    <protectedRange name="p1dea20de3ec8c8e2f76cb4ad76361bd4" sqref="A25:S25" password="C724"/>
+    <protectedRange name="pbda8050ade121dab1a9fdd0b7294aac2" sqref="A26:S26" password="C724"/>
+    <protectedRange name="p05a9a1547c0eeab72d7f056bc566b905" sqref="A27:S27" password="C724"/>
+    <protectedRange name="pd0e8cbfe167f62a09ff9aeadc46bb2cf" sqref="A28:S28" password="C724"/>
+    <protectedRange name="p251c45d3b684b261b9e0e522aa357d5c" sqref="A29:S29" password="C724"/>
+    <protectedRange name="pfc490ec25abad0f8349ad0e74f359b03" sqref="A30:S30" password="C724"/>
+    <protectedRange name="p73b8d239af84e6f1c3a7e245ddad8e05" sqref="A31:S31" password="C724"/>
+    <protectedRange name="p172b5895025b324a3c548a088a8dfaca" sqref="A32:S32" password="C724"/>
+    <protectedRange name="p716a9a2d1741c4db0cb09c2aec52db29" sqref="A33:S33" password="C724"/>
+    <protectedRange name="p9cfbb5c437c241342f7fcd90282a223e" sqref="A34:S34" password="C724"/>
+    <protectedRange name="pd73c4c6890207128eda530126c2cc046" sqref="A35:S35" password="C724"/>
+    <protectedRange name="pcf6bd0cba278dd6ca2a84a3df8acc6fe" sqref="A36:S36" password="C724"/>
+    <protectedRange name="p5da6109c665fe16ea6e23a5b499c6b87" sqref="A37:S37" password="C724"/>
+    <protectedRange name="p771826f70c2ae0720d5733547734bf13" sqref="A38:S38" password="C724"/>
+    <protectedRange name="p431c55b23b26f83950251b61c57285c4" sqref="A39:S39" password="C724"/>
   </protectedRanges>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add rack list and rack field in encoding
</commit_message>
<xml_diff>
--- a/Equipment Tools.xlsx
+++ b/Equipment Tools.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
   <si>
     <t>Equipment and Tools Fields</t>
   </si>
@@ -65,6 +65,9 @@
     <t>Company</t>
   </si>
   <si>
+    <t>Rack</t>
+  </si>
+  <si>
     <t>Physical Condition</t>
   </si>
   <si>
@@ -80,16 +83,10 @@
     <t>Furniture, Fixtures and Equipment</t>
   </si>
   <si>
-    <t>FFE- COMP-BCD-1002</t>
-  </si>
-  <si>
-    <t>Computer</t>
-  </si>
-  <si>
-    <t>AOC</t>
-  </si>
-  <si>
-    <t>1234wq1</t>
+    <t>FFE- COMP-BCD-1004</t>
+  </si>
+  <si>
+    <t>TESTING AGAIN</t>
   </si>
   <si>
     <t>pc/s</t>
@@ -104,22 +101,10 @@
     <t>IT Department</t>
   </si>
   <si>
-    <t>4500.00 PHP</t>
-  </si>
-  <si>
-    <t>4500 PHP</t>
-  </si>
-  <si>
-    <t>FFE- COMP-BCD-1001</t>
-  </si>
-  <si>
-    <t>E2070SWNE</t>
-  </si>
-  <si>
-    <t>5000.00 PHP</t>
-  </si>
-  <si>
-    <t>5000 PHP</t>
+    <t xml:space="preserve">0.00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 </t>
   </si>
 </sst>
 </file>
@@ -505,7 +490,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,9 +501,9 @@
     <col min="1" max="1" width="39.990234" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="22.280273" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="15.996094" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="15.996094" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="16.424561" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="5.570068" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="11.711426" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="5.570068" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="10.283203" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="5.855713" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="5.855713" bestFit="true" customWidth="true" style="0"/>
@@ -528,13 +513,14 @@
     <col min="13" max="13" width="18.852539" bestFit="true" customWidth="true" style="0"/>
     <col min="14" max="14" width="9.283447" bestFit="true" customWidth="true" style="0"/>
     <col min="15" max="15" width="7.426758" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="17.852783" bestFit="true" customWidth="true" style="0"/>
-    <col min="17" max="17" width="13.996582" bestFit="true" customWidth="true" style="0"/>
-    <col min="18" max="18" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="19" max="19" width="7.426758" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="4.570313" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="17.852783" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="9.283447" bestFit="true" customWidth="true" style="0"/>
+    <col min="19" max="19" width="10.283203" bestFit="true" customWidth="true" style="0"/>
+    <col min="20" max="20" width="7.426758" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:20">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -542,7 +528,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:20">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -600,102 +586,56 @@
       <c r="S2" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="T2" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:20">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="2">
         <v>1</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="3" t="s">
+      <c r="Q3" s="1"/>
+      <c r="R3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="S3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="R3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="S3" s="1"/>
-    </row>
-    <row r="4" spans="1:19">
-      <c r="A4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="2">
-        <v>1</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="S4" s="1"/>
+      <c r="T3" s="1"/>
     </row>
   </sheetData>
   <sheetProtection sheet="true" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <protectedRanges>
-    <protectedRange name="p6f5710c8199129451d13d7cdd4fbfe8e" sqref="A3:S3" password="C724"/>
-    <protectedRange name="p5789a9ca630561449388a885f4dbc751" sqref="A4:S4" password="C724"/>
+    <protectedRange name="p9bf551c607ca85b45fc3f030fc4dcdda" sqref="A3:T3" password="C724"/>
   </protectedRanges>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add lost Items Function
</commit_message>
<xml_diff>
--- a/Equipment Tools.xlsx
+++ b/Equipment Tools.xlsx
@@ -80,25 +80,25 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>Furniture, Fixtures and Equipment</t>
-  </si>
-  <si>
-    <t>FFE- COMP-BCD-1004</t>
-  </si>
-  <si>
-    <t>TESTING AGAIN</t>
-  </si>
-  <si>
-    <t>pc/s</t>
-  </si>
-  <si>
-    <t>Stephine David Severino</t>
+    <t>Furniture, Fixtures and Equipment-CPGC</t>
+  </si>
+  <si>
+    <t>FFE-FUR-CPGC-1030</t>
+  </si>
+  <si>
+    <t>ste</t>
+  </si>
+  <si>
+    <t>drum/s</t>
+  </si>
+  <si>
+    <t>Jan Lester Mercene Madriaga</t>
   </si>
   <si>
     <t>Assigned</t>
   </si>
   <si>
-    <t>IT Department</t>
+    <t>Operations</t>
   </si>
   <si>
     <t xml:space="preserve">0.00 </t>
@@ -498,17 +498,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="39.990234" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="22.280273" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="45.845947" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="21.137695" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="15.996094" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="16.424561" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="15.996094" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="5.570068" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="5.570068" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="10.283203" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="5.855713" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="5.855713" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="8.140869" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="12.139893" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="28.135986" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="32.991943" bestFit="true" customWidth="true" style="0"/>
     <col min="12" max="12" width="10.568848" bestFit="true" customWidth="true" style="0"/>
     <col min="13" max="13" width="18.852539" bestFit="true" customWidth="true" style="0"/>
     <col min="14" max="14" width="9.283447" bestFit="true" customWidth="true" style="0"/>

</xml_diff>